<commit_message>
Footprint added and began LTC4015 layout
Created LTC4015 footprint in library and schematic. Updated BOM for original board with prices for each part and consolidated parts
</commit_message>
<xml_diff>
--- a/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
+++ b/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
@@ -7,67 +7,40 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="20115" windowHeight="9030"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="2017-06-07T13-52-05" sheetId="5" r:id="rId2"/>
     <sheet name="2017-06-06T19-29-56" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$35</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="246">
   <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>HEADER-1X8ROUND</t>
-  </si>
-  <si>
-    <t>1X08_ROUND</t>
-  </si>
-  <si>
-    <t>JP10</t>
-  </si>
-  <si>
-    <t>PIN HEADER</t>
-  </si>
-  <si>
     <t>JST_2PIN-SMT-RA</t>
   </si>
   <si>
     <t>JST-PH-2-SMT-RA</t>
   </si>
   <si>
-    <t>BATT, BATT1, LOAD, LOAD1</t>
-  </si>
-  <si>
     <t>JST 2-Pin Connectors of various flavors</t>
   </si>
   <si>
-    <t>PINHD-1X3CB</t>
-  </si>
-  <si>
-    <t>1X03-CLEANBIG</t>
-  </si>
-  <si>
-    <t>JP5, JP8</t>
-  </si>
-  <si>
     <t>TERMBLOCK_1X2</t>
   </si>
   <si>
     <t>TERMBLOCK_1X2-3.5MM</t>
   </si>
   <si>
-    <t>X1, X2</t>
-  </si>
-  <si>
     <t>3.5mm Terminal block</t>
   </si>
   <si>
@@ -173,9 +146,6 @@
     <t>C0805K</t>
   </si>
   <si>
-    <t>C1, C2, C3, C5, C6, C7</t>
-  </si>
-  <si>
     <t>CAP_CERAMIC0805-NOOUTLINE</t>
   </si>
   <si>
@@ -263,18 +233,6 @@
     <t>R37</t>
   </si>
   <si>
-    <t>BATT</t>
-  </si>
-  <si>
-    <t>HEADER-1X2ROUND</t>
-  </si>
-  <si>
-    <t>1X02_ROUND</t>
-  </si>
-  <si>
-    <t>JP4, JP7</t>
-  </si>
-  <si>
     <t>BLUE</t>
   </si>
   <si>
@@ -290,30 +248,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>DCIN</t>
-  </si>
-  <si>
-    <t>DCBARRELSMT</t>
-  </si>
-  <si>
-    <t>DCJACK_2MM_SMT</t>
-  </si>
-  <si>
-    <t>CN1</t>
-  </si>
-  <si>
-    <t>DC Barrel Jack</t>
-  </si>
-  <si>
-    <t>HEADER-1X2</t>
-  </si>
-  <si>
-    <t>1X02_OVAL</t>
-  </si>
-  <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
     <t>FIDUCIAL</t>
   </si>
   <si>
@@ -332,12 +266,6 @@
     <t>DONE, DONE1</t>
   </si>
   <si>
-    <t>LOAD</t>
-  </si>
-  <si>
-    <t>JP3, JP6</t>
-  </si>
-  <si>
     <t>MBR120VLSFT1G</t>
   </si>
   <si>
@@ -377,21 +305,6 @@
     <t>PNP Bias Resistor Transistor</t>
   </si>
   <si>
-    <t>MOUNTINGHOLE2</t>
-  </si>
-  <si>
-    <t>.5 MOUNTINGHOLE2.5</t>
-  </si>
-  <si>
-    <t>MOUNTINGHOLE_2.5_PLATED</t>
-  </si>
-  <si>
-    <t>U$4, U$5, U$6, U$7</t>
-  </si>
-  <si>
-    <t>Mounting Hole</t>
-  </si>
-  <si>
     <t>MicroUSB</t>
   </si>
   <si>
@@ -782,9 +695,6 @@
     <t>Part # and device do not match but 2133 PNP should work fine</t>
   </si>
   <si>
-    <t>Mounting hole N/A</t>
-  </si>
-  <si>
     <t>FIDUCIAL N/A</t>
   </si>
   <si>
@@ -804,13 +714,61 @@
   </si>
   <si>
     <t>R7, R8, R9, R10, R13, R14, R11, R15, R39, R40</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Extended Price</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>BATT, BATT1</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C5, C6, C7, C15</t>
+  </si>
+  <si>
+    <t>609-4946-1-ND</t>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+  </si>
+  <si>
+    <t>87583-3010RPALF</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>S2B-PH-K-S(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1719-ND</t>
+  </si>
+  <si>
+    <t>3.7 - 4.2 V</t>
+  </si>
+  <si>
+    <t>732-2745-ND</t>
+  </si>
+  <si>
+    <t>Wurth Electronics Inc.</t>
+  </si>
+  <si>
+    <t>2POS HORIZ 3.5MM T/H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,6 +838,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -902,7 +899,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -947,6 +944,34 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1256,784 +1281,979 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" customWidth="1"/>
-    <col min="11" max="11" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="47.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="G2" s="17">
+        <f>E2*F2</f>
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="2">
+        <v>691103110002</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="F3" s="17">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="G3" s="17">
+        <f>E3*F3</f>
+        <v>0.56420000000000003</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" t="str">
+        <f>VLOOKUP(K3,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 10UF 16V X5R 0805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G4" s="17">
+        <f>E4*F4</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" t="str">
+        <f>VLOOKUP(K4,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 100UF 10V X5R 1210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="17">
+        <v>1.67E-2</v>
+      </c>
+      <c r="G5" s="17">
+        <f>E5*F5</f>
+        <v>1.67E-2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="J5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="L5" t="str">
+        <f>VLOOKUP(K5,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 0.1UF 50V Y5V 0805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="24" t="str">
+        <f>VLOOKUP(K6,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 10UF 16V X5R 0805</v>
+      </c>
+      <c r="M6" s="25"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="17">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="G7" s="17">
+        <f>E7*F7</f>
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" t="str">
-        <f>VLOOKUP(I2,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 10UF 16V X5R 0805</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="L7" t="str">
+        <f>VLOOKUP(K7,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 2.2UF 25V X5R 0805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.2437</v>
+      </c>
+      <c r="G8" s="17">
+        <f>E8*F8</f>
+        <v>0.73109999999999997</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" t="str">
+        <f>VLOOKUP(K8,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="M9" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="J3" t="str">
-        <f>VLOOKUP(I3,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="F10" s="17">
+        <v>0.3019</v>
+      </c>
+      <c r="G10" s="17">
+        <f>E10*F10</f>
+        <v>0.3019</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="L10" t="str">
+        <f>VLOOKUP(K10,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="K6" s="14" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="J7" t="str">
-        <f>VLOOKUP(I7,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J8" t="str">
-        <f>VLOOKUP(I8,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 10UF 16V X5R 0805</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="J9" t="str">
-        <f>VLOOKUP(I9,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="J10" t="str">
-        <f>VLOOKUP(I10,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>242</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>197</v>
+      <c r="F11" s="17">
+        <v>9.9099999999999994E-2</v>
+      </c>
+      <c r="G11" s="17">
+        <f>E11*F11</f>
+        <v>0.19819999999999999</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="J11" t="str">
-        <f>VLOOKUP(I11,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED GREEN DIFFUSED 0805 SMD</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>203</v>
+      <c r="F12" s="17">
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" ref="G12:G35" si="0">E12*F12</f>
+        <v>0.18959999999999999</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="J12" t="str">
-        <f>VLOOKUP(I12,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED RED DIFFUSED 0805 SMD</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="L12" t="str">
+        <f>VLOOKUP(K12,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED GREEN DIFFUSED 0805 SMD</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>202</v>
+        <v>99</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>201</v>
+      <c r="F13" s="17">
+        <v>9.98E-2</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
+        <v>0.1996</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="J13" t="str">
-        <f>VLOOKUP(I13,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED YELLOW DIFFUSED 0805 SMD</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="L13" t="str">
+        <f>VLOOKUP(K13,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED RED DIFFUSED 0805 SMD</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>173</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>212</v>
+      <c r="F14" s="17">
+        <v>0.1331</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="0"/>
+        <v>0.26619999999999999</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J14" t="str">
-        <f>VLOOKUP(I14,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="L14" t="str">
+        <f>VLOOKUP(K14,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED YELLOW DIFFUSED 0805 SMD</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="17">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="L15" t="str">
+        <f>VLOOKUP(K15,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED BLUE CLEAR 0805 SMD</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1.5347999999999999</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="0"/>
+        <v>3.0695999999999999</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L16" t="str">
+        <f>VLOOKUP(K16,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="17">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="0"/>
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="L17" t="str">
+        <f>VLOOKUP(K17,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="17">
+        <v>0.62160000000000004</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2432000000000001</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="L18" t="str">
+        <f>VLOOKUP(K18,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" t="str">
-        <f>VLOOKUP(I15,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="1">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" t="str">
-        <f>VLOOKUP(I16,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="1">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="J17" t="str">
-        <f>VLOOKUP(I17,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="1">
-        <v>10</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J18" t="str">
-        <f>VLOOKUP(I18,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>163</v>
+      <c r="F19" s="17">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="J19" t="str">
-        <f>VLOOKUP(I19,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="L19" t="str">
+        <f>VLOOKUP(K19,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>206</v>
+      <c r="F20" s="17">
+        <v>0.60029999999999994</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2005999999999999</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="L20" t="str">
+        <f>VLOOKUP(K20,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="17">
+        <v>0.4304</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="0"/>
+        <v>0.86080000000000001</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" t="str">
+        <f>VLOOKUP(K21,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="1">
         <v>4</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>206</v>
+      <c r="F22" s="17">
+        <v>1.29E-2</v>
+      </c>
+      <c r="G22" s="17">
+        <f t="shared" si="0"/>
+        <v>5.16E-2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>206</v>
+        <v>28</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L22" t="str">
+        <f>VLOOKUP(K22,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="E23" s="1">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>206</v>
+        <v>10</v>
+      </c>
+      <c r="F23" s="17">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="G23" s="17">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L23" t="str">
+        <f>VLOOKUP(K23,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>206</v>
+      <c r="F24" s="17">
+        <v>7.9899999999999999E-2</v>
+      </c>
+      <c r="G24" s="17">
+        <f t="shared" si="0"/>
+        <v>0.1598</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>206</v>
+        <v>53</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="L24" t="str">
+        <f>VLOOKUP(K24,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
@@ -2042,616 +2262,457 @@
         <v>25</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="17">
+        <v>1.67E-2</v>
+      </c>
+      <c r="G25" s="17">
+        <f t="shared" si="0"/>
+        <v>1.67E-2</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="I25" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I25" s="6" t="s">
+      <c r="J25" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K25" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="J25" t="str">
-        <f>VLOOKUP(I25,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 0.1UF 50V Y5V 0805</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L25" t="str">
+        <f>VLOOKUP(K25,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>179</v>
+      <c r="F26" s="17">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G26" s="17">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="J26" t="str">
-        <f>VLOOKUP(I26,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 100UF 10V X5R 1210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="L26" t="str">
+        <f>VLOOKUP(K26,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>183</v>
+      <c r="F27" s="17">
+        <v>1.67E-2</v>
+      </c>
+      <c r="G27" s="17">
+        <f t="shared" si="0"/>
+        <v>1.67E-2</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="J27" t="str">
-        <f>VLOOKUP(I27,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 2.2UF 25V X5R 0805</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="L27" t="str">
+        <f>VLOOKUP(K27,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>188</v>
+        <v>2</v>
+      </c>
+      <c r="F28" s="17">
+        <v>1.29E-2</v>
+      </c>
+      <c r="G28" s="17">
+        <f t="shared" si="0"/>
+        <v>2.58E-2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="J28" t="str">
-        <f>VLOOKUP(I28,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="L28" t="str">
+        <f>VLOOKUP(K28,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>132</v>
+        <v>21</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>130</v>
+      <c r="F29" s="17">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="J29" t="str">
-        <f>VLOOKUP(I29,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="L29" t="str">
+        <f>VLOOKUP(K29,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="17">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="G30" s="17">
+        <f t="shared" si="0"/>
+        <v>8.8800000000000004E-2</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="L30" t="str">
+        <f>VLOOKUP(K30,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="17">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="G31" s="17">
+        <f t="shared" si="0"/>
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="L31" t="str">
+        <f>VLOOKUP(K31,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="17">
+        <v>1.7770999999999999</v>
+      </c>
+      <c r="G32" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7770999999999999</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="L32" t="str">
+        <f>VLOOKUP(K32,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
         <v>IC REG BOOST ADJ 2A SYNC 16VQFN</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J30" t="str">
-        <f>VLOOKUP(I30,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED BLUE CLEAR 0805 SMD</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="1">
-        <v>2</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="J31" t="str">
-        <f>VLOOKUP(I31,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="J32" t="str">
-        <f>VLOOKUP(I32,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>170</v>
+      <c r="F33" s="17">
+        <v>0.65680000000000005</v>
+      </c>
+      <c r="G33" s="17">
+        <f t="shared" si="0"/>
+        <v>0.65680000000000005</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J33" t="str">
-        <f>VLOOKUP(I33,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
+        <v>109</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>172</v>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="J34" t="str">
-        <f>VLOOKUP(I34,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
+        <v>97</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
-        <v>2</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>174</v>
+        <v>1</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="J35" t="str">
-        <f>VLOOKUP(I35,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="J36" t="str">
-        <f>VLOOKUP(I36,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" s="1">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="J37" t="str">
-        <f>VLOOKUP(I37,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="1">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="1">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E42" s="1">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>206</v>
+        <v>9</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K42">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="R11, R15"/>
-        <filter val="R2, R4"/>
-        <filter val="R3, R6, R12, R16"/>
-        <filter val="R35"/>
-        <filter val="R36, R38"/>
-        <filter val="R37"/>
-        <filter val="R39, R40"/>
-        <filter val="R41, R43"/>
-        <filter val="R42"/>
-        <filter val="R44"/>
-        <filter val="R45"/>
-        <filter val="R5, R17"/>
-        <filter val="R7, R8, R9, R10, R13, R14"/>
-        <filter val="RT1, RT2"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A3:K38">
-      <sortCondition ref="D1:D44"/>
+  <autoFilter ref="A1:M35">
+    <sortState ref="A2:K42">
+      <sortCondition ref="A1:A42"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="I18" r:id="rId1"/>
-    <hyperlink ref="I16" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
-    <hyperlink ref="I17" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
-    <hyperlink ref="I19" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
-    <hyperlink ref="I32" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
-    <hyperlink ref="I31" r:id="rId6" display=" CR0805-FX-2003ELFCT-ND"/>
-    <hyperlink ref="I33" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
-    <hyperlink ref="I34" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
-    <hyperlink ref="I35" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
-    <hyperlink ref="I36" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
-    <hyperlink ref="I26" r:id="rId11" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM32ER61A107ME20L/490-9969-1-ND/5026474"/>
-    <hyperlink ref="I2" r:id="rId12"/>
-    <hyperlink ref="I25" r:id="rId13" display="https://www.digikey.com/product-detail/en/yageo/CC0805ZRY5V9BB104/311-1361-1-ND/2103145"/>
-    <hyperlink ref="I27" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
-    <hyperlink ref="I7" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
-    <hyperlink ref="I28" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
-    <hyperlink ref="I9" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
-    <hyperlink ref="I11" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
-    <hyperlink ref="I12" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
-    <hyperlink ref="I13" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
-    <hyperlink ref="I30" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
-    <hyperlink ref="I10" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
-    <hyperlink ref="I29" r:id="rId23"/>
-    <hyperlink ref="I3" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="I15" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="I14" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
-    <hyperlink ref="I37" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
-    <hyperlink ref="I8" r:id="rId28"/>
+    <hyperlink ref="K23" r:id="rId1"/>
+    <hyperlink ref="K22" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
+    <hyperlink ref="K20" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
+    <hyperlink ref="K21" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
+    <hyperlink ref="K24" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
+    <hyperlink ref="K28" r:id="rId6"/>
+    <hyperlink ref="K26" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
+    <hyperlink ref="K29" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
+    <hyperlink ref="K30" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
+    <hyperlink ref="K31" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
+    <hyperlink ref="K4" r:id="rId11" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM32ER61A107ME20L/490-9969-1-ND/5026474"/>
+    <hyperlink ref="K3" r:id="rId12"/>
+    <hyperlink ref="K5" r:id="rId13" display="https://www.digikey.com/product-detail/en/yageo/CC0805ZRY5V9BB104/311-1361-1-ND/2103145"/>
+    <hyperlink ref="K7" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
+    <hyperlink ref="K18" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
+    <hyperlink ref="K10" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
+    <hyperlink ref="K8" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
+    <hyperlink ref="K12" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
+    <hyperlink ref="K13" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
+    <hyperlink ref="K14" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
+    <hyperlink ref="K15" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
+    <hyperlink ref="K16" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
+    <hyperlink ref="K32" r:id="rId23"/>
+    <hyperlink ref="K27" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K25" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K19" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
+    <hyperlink ref="K17" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
+    <hyperlink ref="K6" r:id="rId28"/>
+    <hyperlink ref="K33" r:id="rId29"/>
+    <hyperlink ref="K11" r:id="rId30"/>
+    <hyperlink ref="K2" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -2670,31 +2731,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="F1" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G1" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="H1" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="I1" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2705,10 +2766,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -2731,10 +2792,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -2757,10 +2818,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -2783,10 +2844,10 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -2809,10 +2870,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -2835,10 +2896,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -2861,10 +2922,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -2887,10 +2948,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" t="s">
         <v>200</v>
-      </c>
-      <c r="D9" t="s">
-        <v>229</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -2913,10 +2974,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -2939,10 +3000,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -2965,10 +3026,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -2991,10 +3052,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" t="s">
         <v>204</v>
-      </c>
-      <c r="D13" t="s">
-        <v>233</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3017,10 +3078,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3043,10 +3104,10 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3069,10 +3130,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3095,10 +3156,10 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3121,10 +3182,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3147,10 +3208,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3173,10 +3234,10 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3199,10 +3260,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3225,10 +3286,10 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -3251,10 +3312,10 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -3277,10 +3338,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -3303,10 +3364,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -3329,10 +3390,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="D26" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -3355,10 +3416,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="F27">
         <v>10</v>
@@ -3381,10 +3442,10 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="D28" t="s">
-        <v>255</v>
+        <v>225</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -3407,10 +3468,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
       <c r="D29" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="F29">
         <v>10</v>
@@ -3448,31 +3509,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="F1" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="G1" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="H1" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="I1" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3483,10 +3544,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -3509,10 +3570,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -3535,10 +3596,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -3561,10 +3622,10 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -3587,10 +3648,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>151</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>197</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -3613,10 +3674,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>198</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -3639,10 +3700,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>228</v>
+        <v>199</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -3665,10 +3726,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" t="s">
         <v>200</v>
-      </c>
-      <c r="D9" t="s">
-        <v>229</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -3691,10 +3752,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>170</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -3717,10 +3778,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -3743,10 +3804,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>203</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3769,10 +3830,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
+        <v>175</v>
+      </c>
+      <c r="D13" t="s">
         <v>204</v>
-      </c>
-      <c r="D13" t="s">
-        <v>233</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3795,10 +3856,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3821,10 +3882,10 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3847,10 +3908,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3873,10 +3934,10 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3899,10 +3960,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3925,10 +3986,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3951,10 +4012,10 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3977,10 +4038,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="D21" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -4003,10 +4064,10 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -4029,10 +4090,10 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -4055,10 +4116,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -4081,10 +4142,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -4107,10 +4168,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>178</v>
       </c>
       <c r="D26" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -4133,10 +4194,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="F27">
         <v>10</v>

</xml_diff>

<commit_message>
Updated BOM for master repo
BOM updated to match board layout and added prices
</commit_message>
<xml_diff>
--- a/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
+++ b/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
@@ -7,82 +7,43 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="20115" windowHeight="9030"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="2017-06-07T13-52-05" sheetId="5" r:id="rId2"/>
     <sheet name="2017-06-06T19-29-56" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$33</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="238">
   <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>HEADER-1X8ROUND</t>
-  </si>
-  <si>
-    <t>1X08_ROUND</t>
-  </si>
-  <si>
-    <t>JP10</t>
-  </si>
-  <si>
-    <t>PIN HEADER</t>
-  </si>
-  <si>
     <t>JST_2PIN-SMT-RA</t>
   </si>
   <si>
     <t>JST-PH-2-SMT-RA</t>
   </si>
   <si>
-    <t>BATT, BATT1, LOAD, LOAD1</t>
-  </si>
-  <si>
     <t>JST 2-Pin Connectors of various flavors</t>
   </si>
   <si>
-    <t>PINHD-1X3CB</t>
-  </si>
-  <si>
-    <t>1X03-CLEANBIG</t>
-  </si>
-  <si>
-    <t>JP5, JP8</t>
-  </si>
-  <si>
     <t>TERMBLOCK_1X2</t>
   </si>
   <si>
     <t>TERMBLOCK_1X2-3.5MM</t>
   </si>
   <si>
-    <t>X1, X2</t>
-  </si>
-  <si>
     <t>3.5mm Terminal block</t>
   </si>
   <si>
-    <t>USBMINIBLARGE</t>
-  </si>
-  <si>
-    <t>USB-MINIB_LARGER</t>
-  </si>
-  <si>
-    <t>CN4</t>
-  </si>
-  <si>
-    <t>USB Connectors</t>
-  </si>
-  <si>
     <t>R-US_R0805</t>
   </si>
   <si>
@@ -173,9 +134,6 @@
     <t>C0805K</t>
   </si>
   <si>
-    <t>C1, C2, C3, C5, C6, C7</t>
-  </si>
-  <si>
     <t>CAP_CERAMIC0805-NOOUTLINE</t>
   </si>
   <si>
@@ -263,18 +221,6 @@
     <t>R37</t>
   </si>
   <si>
-    <t>BATT</t>
-  </si>
-  <si>
-    <t>HEADER-1X2ROUND</t>
-  </si>
-  <si>
-    <t>1X02_ROUND</t>
-  </si>
-  <si>
-    <t>JP4, JP7</t>
-  </si>
-  <si>
     <t>BLUE</t>
   </si>
   <si>
@@ -290,30 +236,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>DCIN</t>
-  </si>
-  <si>
-    <t>DCBARRELSMT</t>
-  </si>
-  <si>
-    <t>DCJACK_2MM_SMT</t>
-  </si>
-  <si>
-    <t>CN1</t>
-  </si>
-  <si>
-    <t>DC Barrel Jack</t>
-  </si>
-  <si>
-    <t>HEADER-1X2</t>
-  </si>
-  <si>
-    <t>1X02_OVAL</t>
-  </si>
-  <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
     <t>FIDUCIAL</t>
   </si>
   <si>
@@ -332,12 +254,6 @@
     <t>DONE, DONE1</t>
   </si>
   <si>
-    <t>LOAD</t>
-  </si>
-  <si>
-    <t>JP3, JP6</t>
-  </si>
-  <si>
     <t>MBR120VLSFT1G</t>
   </si>
   <si>
@@ -377,33 +293,6 @@
     <t>PNP Bias Resistor Transistor</t>
   </si>
   <si>
-    <t>MOUNTINGHOLE2</t>
-  </si>
-  <si>
-    <t>.5 MOUNTINGHOLE2.5</t>
-  </si>
-  <si>
-    <t>MOUNTINGHOLE_2.5_PLATED</t>
-  </si>
-  <si>
-    <t>U$4, U$5, U$6, U$7</t>
-  </si>
-  <si>
-    <t>Mounting Hole</t>
-  </si>
-  <si>
-    <t>MicroUSB</t>
-  </si>
-  <si>
-    <t>USBMICRO_20329</t>
-  </si>
-  <si>
-    <t>4UCONN_20329</t>
-  </si>
-  <si>
-    <t>CN6</t>
-  </si>
-  <si>
     <t>CHRG/LBO, CHRG/LBO1</t>
   </si>
   <si>
@@ -782,9 +671,6 @@
     <t>Part # and device do not match but 2133 PNP should work fine</t>
   </si>
   <si>
-    <t>Mounting hole N/A</t>
-  </si>
-  <si>
     <t>FIDUCIAL N/A</t>
   </si>
   <si>
@@ -804,13 +690,61 @@
   </si>
   <si>
     <t>R7, R8, R9, R10, R13, R14, R11, R15, R39, R40</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Extended Price</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>BATT, BATT1</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C5, C6, C7, C15</t>
+  </si>
+  <si>
+    <t>609-4946-1-ND</t>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+  </si>
+  <si>
+    <t>87583-3010RPALF</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>S2B-PH-K-S(LF)(SN)</t>
+  </si>
+  <si>
+    <t>455-1719-ND</t>
+  </si>
+  <si>
+    <t>3.7 - 4.2 V</t>
+  </si>
+  <si>
+    <t>732-2745-ND</t>
+  </si>
+  <si>
+    <t>Wurth Electronics Inc.</t>
+  </si>
+  <si>
+    <t>2POS HORIZ 3.5MM T/H</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,6 +814,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -902,7 +875,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -947,6 +920,34 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1256,1402 +1257,1373 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="29" style="2" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" customWidth="1"/>
-    <col min="11" max="11" width="47.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="18" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="47.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="G2" s="17">
+        <f>E2*F2</f>
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="I2" s="2">
+        <v>691103110002</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="F3" s="17">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="G3" s="17">
+        <f>E3*F3</f>
+        <v>0.56420000000000003</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" t="str">
+        <f>VLOOKUP(K3,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 10UF 16V X5R 0805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G4" s="17">
+        <f>E4*F4</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="K4" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" t="str">
+        <f>VLOOKUP(K4,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 100UF 10V X5R 1210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="17">
+        <v>1.67E-2</v>
+      </c>
+      <c r="G5" s="17">
+        <f>E5*F5</f>
+        <v>1.67E-2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="L5" t="str">
+        <f>VLOOKUP(K5,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 0.1UF 50V Y5V 0805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="L6" s="24" t="str">
+        <f>VLOOKUP(K6,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 10UF 16V X5R 0805</v>
+      </c>
+      <c r="M6" s="25"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="17">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="G7" s="17">
+        <f>E7*F7</f>
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="L7" t="str">
+        <f>VLOOKUP(K7,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 2.2UF 25V X5R 0805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.2437</v>
+      </c>
+      <c r="G8" s="17">
+        <f>E8*F8</f>
+        <v>0.73109999999999997</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L8" t="str">
+        <f>VLOOKUP(K8,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="M9" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0.3019</v>
+      </c>
+      <c r="G10" s="17">
+        <f>E10*F10</f>
+        <v>0.3019</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="K1" s="12" t="s">
+      <c r="K10" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="L10" t="str">
+        <f>VLOOKUP(K10,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
+      </c>
+      <c r="M10" s="15" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="1">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" t="str">
-        <f>VLOOKUP(I2,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 10UF 16V X5R 0805</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="J3" t="str">
-        <f>VLOOKUP(I3,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="K6" s="14" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="J7" t="str">
-        <f>VLOOKUP(I7,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J8" t="str">
-        <f>VLOOKUP(I8,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 10UF 16V X5R 0805</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="J9" t="str">
-        <f>VLOOKUP(I9,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="J10" t="str">
-        <f>VLOOKUP(I10,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>234</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>197</v>
+      <c r="F11" s="17">
+        <v>9.9099999999999994E-2</v>
+      </c>
+      <c r="G11" s="17">
+        <f>E11*F11</f>
+        <v>0.19819999999999999</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="J11" t="str">
-        <f>VLOOKUP(I11,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED GREEN DIFFUSED 0805 SMD</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>203</v>
+      <c r="F12" s="17">
+        <v>9.4799999999999995E-2</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" ref="G12:G33" si="0">E12*F12</f>
+        <v>0.18959999999999999</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="J12" t="str">
-        <f>VLOOKUP(I12,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED RED DIFFUSED 0805 SMD</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="L12" t="str">
+        <f>VLOOKUP(K12,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED GREEN DIFFUSED 0805 SMD</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>202</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>201</v>
+      <c r="F13" s="17">
+        <v>9.98E-2</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
+        <v>0.1996</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="J13" t="str">
-        <f>VLOOKUP(I13,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED YELLOW DIFFUSED 0805 SMD</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L13" t="str">
+        <f>VLOOKUP(K13,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED RED DIFFUSED 0805 SMD</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>212</v>
+      <c r="F14" s="17">
+        <v>0.1331</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="0"/>
+        <v>0.26619999999999999</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="J14" t="str">
-        <f>VLOOKUP(I14,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="L14" t="str">
+        <f>VLOOKUP(K14,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED YELLOW DIFFUSED 0805 SMD</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>210</v>
+      <c r="F15" s="17">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" t="str">
-        <f>VLOOKUP(I15,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="L15" t="str">
+        <f>VLOOKUP(K15,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED BLUE CLEAR 0805 SMD</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="E16" s="1">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="H16" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="17">
+        <v>1.5347999999999999</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="0"/>
+        <v>3.0695999999999999</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L16" t="str">
+        <f>VLOOKUP(K16,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="17">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="0"/>
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" t="str">
-        <f>VLOOKUP(I16,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="K17" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="L17" t="str">
+        <f>VLOOKUP(K17,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="E18" s="1">
         <v>2</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="J17" t="str">
-        <f>VLOOKUP(I17,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="1">
-        <v>10</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="F18" s="17">
+        <v>0.62160000000000004</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2432000000000001</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="J18" t="str">
-        <f>VLOOKUP(I18,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L18" t="str">
+        <f>VLOOKUP(K18,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>163</v>
+      <c r="F19" s="17">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="J19" t="str">
-        <f>VLOOKUP(I19,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="L19" t="str">
+        <f>VLOOKUP(K19,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>206</v>
+      <c r="F20" s="17">
+        <v>0.60029999999999994</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2005999999999999</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L20" t="str">
+        <f>VLOOKUP(K20,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>206</v>
+      <c r="F21" s="17">
+        <v>0.4304</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="0"/>
+        <v>0.86080000000000001</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="L21" t="str">
+        <f>VLOOKUP(K21,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1">
         <v>4</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>206</v>
+      <c r="F22" s="17">
+        <v>1.29E-2</v>
+      </c>
+      <c r="G22" s="17">
+        <f t="shared" si="0"/>
+        <v>5.16E-2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>206</v>
+        <v>24</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L22" t="str">
+        <f>VLOOKUP(K22,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="E23" s="1">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>206</v>
+        <v>10</v>
+      </c>
+      <c r="F23" s="17">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="G23" s="17">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L23" t="str">
+        <f>VLOOKUP(K23,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>206</v>
+      <c r="F24" s="17">
+        <v>7.9899999999999999E-2</v>
+      </c>
+      <c r="G24" s="17">
+        <f t="shared" si="0"/>
+        <v>0.1598</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>206</v>
+        <v>49</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="L24" t="str">
+        <f>VLOOKUP(K24,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="J25" t="str">
-        <f>VLOOKUP(I25,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 0.1UF 50V Y5V 0805</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="17">
+        <v>1.67E-2</v>
+      </c>
+      <c r="G25" s="17">
+        <f t="shared" si="0"/>
+        <v>1.67E-2</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L25" t="str">
+        <f>VLOOKUP(K25,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>179</v>
+      <c r="F26" s="17">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G26" s="17">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="J26" t="str">
-        <f>VLOOKUP(I26,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 100UF 10V X5R 1210</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="L26" t="str">
+        <f>VLOOKUP(K26,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>183</v>
+      <c r="F27" s="17">
+        <v>1.67E-2</v>
+      </c>
+      <c r="G27" s="17">
+        <f t="shared" si="0"/>
+        <v>1.67E-2</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="J27" t="str">
-        <f>VLOOKUP(I27,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 2.2UF 25V X5R 0805</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="L27" t="str">
+        <f>VLOOKUP(K27,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>188</v>
+        <v>2</v>
+      </c>
+      <c r="F28" s="17">
+        <v>1.29E-2</v>
+      </c>
+      <c r="G28" s="17">
+        <f t="shared" si="0"/>
+        <v>2.58E-2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="J28" t="str">
-        <f>VLOOKUP(I28,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="L28" t="str">
+        <f>VLOOKUP(K28,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>16</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>130</v>
+      <c r="F29" s="17">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" si="0"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="J29" t="str">
-        <f>VLOOKUP(I29,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L29" t="str">
+        <f>VLOOKUP(K29,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="1">
+        <v>2</v>
+      </c>
+      <c r="F30" s="17">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="G30" s="17">
+        <f t="shared" si="0"/>
+        <v>8.8800000000000004E-2</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="L30" t="str">
+        <f>VLOOKUP(K30,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="17">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="G31" s="17">
+        <f t="shared" si="0"/>
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L31" t="str">
+        <f>VLOOKUP(K31,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="17">
+        <v>1.7770999999999999</v>
+      </c>
+      <c r="G32" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7770999999999999</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="L32" t="str">
+        <f>VLOOKUP(K32,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
         <v>IC REG BOOST ADJ 2A SYNC 16VQFN</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J30" t="str">
-        <f>VLOOKUP(I30,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED BLUE CLEAR 0805 SMD</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="1">
-        <v>2</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="J31" t="str">
-        <f>VLOOKUP(I31,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="1">
-        <v>2</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="J32" t="str">
-        <f>VLOOKUP(I32,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>170</v>
+      <c r="F33" s="17">
+        <v>0.65680000000000005</v>
+      </c>
+      <c r="G33" s="17">
+        <f t="shared" si="0"/>
+        <v>0.65680000000000005</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J33" t="str">
-        <f>VLOOKUP(I33,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="J34" t="str">
-        <f>VLOOKUP(I34,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="1">
-        <v>2</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="J35" t="str">
-        <f>VLOOKUP(I35,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="J36" t="str">
-        <f>VLOOKUP(I36,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" s="1">
-        <v>1</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="J37" t="str">
-        <f>VLOOKUP(I37,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="1">
-        <v>1</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="1">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E42" s="1">
-        <v>1</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>206</v>
+        <v>101</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K42">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="R11, R15"/>
-        <filter val="R2, R4"/>
-        <filter val="R3, R6, R12, R16"/>
-        <filter val="R35"/>
-        <filter val="R36, R38"/>
-        <filter val="R37"/>
-        <filter val="R39, R40"/>
-        <filter val="R41, R43"/>
-        <filter val="R42"/>
-        <filter val="R44"/>
-        <filter val="R45"/>
-        <filter val="R5, R17"/>
-        <filter val="R7, R8, R9, R10, R13, R14"/>
-        <filter val="RT1, RT2"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A3:K38">
-      <sortCondition ref="D1:D44"/>
+  <autoFilter ref="A1:M33">
+    <sortState ref="A2:K42">
+      <sortCondition ref="A1:A42"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="I18" r:id="rId1"/>
-    <hyperlink ref="I16" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
-    <hyperlink ref="I17" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
-    <hyperlink ref="I19" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
-    <hyperlink ref="I32" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
-    <hyperlink ref="I31" r:id="rId6" display=" CR0805-FX-2003ELFCT-ND"/>
-    <hyperlink ref="I33" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
-    <hyperlink ref="I34" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
-    <hyperlink ref="I35" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
-    <hyperlink ref="I36" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
-    <hyperlink ref="I26" r:id="rId11" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM32ER61A107ME20L/490-9969-1-ND/5026474"/>
-    <hyperlink ref="I2" r:id="rId12"/>
-    <hyperlink ref="I25" r:id="rId13" display="https://www.digikey.com/product-detail/en/yageo/CC0805ZRY5V9BB104/311-1361-1-ND/2103145"/>
-    <hyperlink ref="I27" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
-    <hyperlink ref="I7" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
-    <hyperlink ref="I28" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
-    <hyperlink ref="I9" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
-    <hyperlink ref="I11" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
-    <hyperlink ref="I12" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
-    <hyperlink ref="I13" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
-    <hyperlink ref="I30" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
-    <hyperlink ref="I10" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
-    <hyperlink ref="I29" r:id="rId23"/>
-    <hyperlink ref="I3" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="I15" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="I14" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
-    <hyperlink ref="I37" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
-    <hyperlink ref="I8" r:id="rId28"/>
+    <hyperlink ref="K23" r:id="rId1"/>
+    <hyperlink ref="K22" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
+    <hyperlink ref="K20" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
+    <hyperlink ref="K21" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
+    <hyperlink ref="K24" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
+    <hyperlink ref="K28" r:id="rId6"/>
+    <hyperlink ref="K26" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
+    <hyperlink ref="K29" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
+    <hyperlink ref="K30" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
+    <hyperlink ref="K31" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
+    <hyperlink ref="K4" r:id="rId11" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM32ER61A107ME20L/490-9969-1-ND/5026474"/>
+    <hyperlink ref="K3" r:id="rId12"/>
+    <hyperlink ref="K5" r:id="rId13" display="https://www.digikey.com/product-detail/en/yageo/CC0805ZRY5V9BB104/311-1361-1-ND/2103145"/>
+    <hyperlink ref="K7" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
+    <hyperlink ref="K18" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
+    <hyperlink ref="K10" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
+    <hyperlink ref="K8" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
+    <hyperlink ref="K12" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
+    <hyperlink ref="K13" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
+    <hyperlink ref="K14" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
+    <hyperlink ref="K15" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
+    <hyperlink ref="K16" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
+    <hyperlink ref="K32" r:id="rId23"/>
+    <hyperlink ref="K27" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K25" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K19" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
+    <hyperlink ref="K17" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
+    <hyperlink ref="K6" r:id="rId28"/>
+    <hyperlink ref="K33" r:id="rId29"/>
+    <hyperlink ref="K11" r:id="rId30"/>
+    <hyperlink ref="K2" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -2670,31 +2642,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="F1" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="G1" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
       <c r="H1" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="I1" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2705,10 +2677,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -2731,10 +2703,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -2757,10 +2729,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -2783,10 +2755,10 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -2809,10 +2781,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -2835,10 +2807,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -2861,10 +2833,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -2887,10 +2859,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -2913,10 +2885,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>193</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -2939,10 +2911,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -2965,10 +2937,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>195</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -2991,10 +2963,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
       <c r="D13" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3017,10 +2989,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3043,10 +3015,10 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3069,10 +3041,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3095,10 +3067,10 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3121,10 +3093,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3147,10 +3119,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3173,10 +3145,10 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3199,10 +3171,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3225,10 +3197,10 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -3251,10 +3223,10 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -3277,10 +3249,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -3303,10 +3275,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -3329,10 +3301,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="D26" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -3355,10 +3327,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="F27">
         <v>10</v>
@@ -3381,10 +3353,10 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="D28" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -3407,10 +3379,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="D29" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="F29">
         <v>10</v>
@@ -3448,31 +3420,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="F1" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="G1" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
       <c r="H1" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="I1" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3483,10 +3455,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -3509,10 +3481,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -3535,10 +3507,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -3561,10 +3533,10 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -3587,10 +3559,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -3613,10 +3585,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -3639,10 +3611,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -3665,10 +3637,10 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -3691,10 +3663,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>193</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -3717,10 +3689,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -3743,10 +3715,10 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>232</v>
+        <v>195</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3769,10 +3741,10 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
       <c r="D13" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3795,10 +3767,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3821,10 +3793,10 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3847,10 +3819,10 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3873,10 +3845,10 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3899,10 +3871,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="D18" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3925,10 +3897,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3951,10 +3923,10 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3977,10 +3949,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -4003,10 +3975,10 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -4029,10 +4001,10 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -4055,10 +4027,10 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -4081,10 +4053,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -4107,10 +4079,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="D26" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -4133,10 +4105,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="F27">
         <v>10</v>

</xml_diff>

<commit_message>
BOM additions and adjustments
Added vertical USB-A female receptacle
</commit_message>
<xml_diff>
--- a/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
+++ b/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="241">
   <si>
     <t>Qty</t>
   </si>
@@ -530,9 +530,6 @@
     <t>MCP73871-2CCI/ML</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>296-15259-1-ND</t>
   </si>
   <si>
@@ -686,9 +683,6 @@
     <t>75K</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
     <t>R7, R8, R9, R10, R13, R14, R11, R15, R39, R40</t>
   </si>
   <si>
@@ -735,6 +729,21 @@
   </si>
   <si>
     <t>2POS HORIZ 3.5MM T/H</t>
+  </si>
+  <si>
+    <t>USB - Type A Connector Vertical</t>
+  </si>
+  <si>
+    <t>ED3074-ND</t>
+  </si>
+  <si>
+    <t>On Shore Technology Inc.</t>
+  </si>
+  <si>
+    <t>CONN USB TYPE A VERTICAL WHITE</t>
+  </si>
+  <si>
+    <t>CN5 optional component for vertical mounting</t>
   </si>
 </sst>
 </file>
@@ -744,7 +753,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,45 +823,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -875,7 +845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -931,23 +901,10 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1259,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1233,7 @@
     <col min="9" max="9" width="21.42578125" style="2" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="26.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" style="20" customWidth="1"/>
     <col min="13" max="13" width="47.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1297,10 +1254,10 @@
         <v>0</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>103</v>
@@ -1314,1242 +1271,1238 @@
       <c r="K1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>212</v>
+      <c r="L1" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="17">
-        <v>0.57099999999999995</v>
+        <v>1.67E-2</v>
       </c>
       <c r="G2" s="17">
-        <f>E2*F2</f>
-        <v>0.57099999999999995</v>
+        <f t="shared" ref="G2:G23" si="0">E2*F2</f>
+        <v>1.67E-2</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="I2" s="2">
-        <v>691103110002</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>236</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>235</v>
+        <v>143</v>
+      </c>
+      <c r="L2" s="20" t="str">
+        <f>VLOOKUP(K2,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>CAP CER 0.1UF 50V Y5V 0805</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F3" s="17">
-        <v>8.0600000000000005E-2</v>
+        <v>1.67E-2</v>
       </c>
       <c r="G3" s="17">
-        <f>E3*F3</f>
-        <v>0.56420000000000003</v>
+        <f t="shared" si="0"/>
+        <v>1.67E-2</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L3" t="str">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="L3" s="20" t="str">
         <f>VLOOKUP(K3,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 10UF 16V X5R 0805</v>
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="17">
-        <v>0.57999999999999996</v>
+        <v>1.67E-2</v>
       </c>
       <c r="G4" s="17">
-        <f>E4*F4</f>
-        <v>0.57999999999999996</v>
+        <f t="shared" si="0"/>
+        <v>1.67E-2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="L4" t="str">
+        <v>128</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" s="20" t="str">
         <f>VLOOKUP(K4,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 100UF 10V X5R 1210</v>
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="17">
+        <v>1.29E-2</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="0"/>
+        <v>5.16E-2</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L5" s="20" t="str">
+        <f>VLOOKUP(K5,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="17">
-        <v>1.67E-2</v>
-      </c>
-      <c r="G5" s="17">
-        <f>E5*F5</f>
-        <v>1.67E-2</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="L5" t="str">
-        <f>VLOOKUP(K5,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 0.1UF 50V Y5V 0805</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="20">
-        <v>1</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="L6" s="24" t="str">
+      <c r="F6" s="17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="L6" s="20" t="str">
         <f>VLOOKUP(K6,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 10UF 16V X5R 0805</v>
-      </c>
-      <c r="M6" s="25"/>
+        <v>CAP CER 100UF 10V X5R 1210</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="17">
-        <v>3.9399999999999998E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="G7" s="17">
-        <f>E7*F7</f>
-        <v>3.9399999999999998E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="L7" t="str">
+        <v>116</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="L7" s="20" t="str">
         <f>VLOOKUP(K7,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 2.2UF 25V X5R 0805</v>
+        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F8" s="17">
-        <v>0.2437</v>
+        <v>8.0600000000000005E-2</v>
       </c>
       <c r="G8" s="17">
-        <f>E8*F8</f>
-        <v>0.73109999999999997</v>
+        <f t="shared" si="0"/>
+        <v>0.56420000000000003</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>154</v>
+        <v>225</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L8" t="str">
+        <v>110</v>
+      </c>
+      <c r="L8" s="20" t="str">
         <f>VLOOKUP(K8,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
+        <v>CAP CER 10UF 16V X5R 0805</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1">
-        <v>3</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.60029999999999994</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2005999999999999</v>
+      </c>
       <c r="H9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="M9" s="14" t="s">
-        <v>216</v>
+        <v>41</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="20" t="str">
+        <f>VLOOKUP(K9,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="17">
-        <v>0.3019</v>
+        <v>0.4304</v>
       </c>
       <c r="G10" s="17">
-        <f>E10*F10</f>
-        <v>0.3019</v>
+        <f t="shared" si="0"/>
+        <v>0.86080000000000001</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>151</v>
+        <v>43</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>126</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="L10" t="str">
+        <v>116</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" s="20" t="str">
         <f>VLOOKUP(K10,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>213</v>
+        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>234</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F11" s="17">
-        <v>9.9099999999999994E-2</v>
+        <v>8.6999999999999994E-3</v>
       </c>
       <c r="G11" s="17">
-        <f>E11*F11</f>
-        <v>0.19819999999999999</v>
+        <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>231</v>
+        <v>113</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>233</v>
+        <v>112</v>
+      </c>
+      <c r="L11" s="20" t="str">
+        <f>VLOOKUP(K11,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="17">
-        <v>9.4799999999999995E-2</v>
+        <v>3.9399999999999998E-2</v>
       </c>
       <c r="G12" s="17">
-        <f t="shared" ref="G12:G33" si="0">E12*F12</f>
-        <v>0.18959999999999999</v>
+        <f t="shared" si="0"/>
+        <v>3.9399999999999998E-2</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="L12" t="str">
+        <v>145</v>
+      </c>
+      <c r="L12" s="20" t="str">
         <f>VLOOKUP(K12,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED GREEN DIFFUSED 0805 SMD</v>
+        <v>CAP CER 2.2UF 25V X5R 0805</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="17">
-        <v>9.98E-2</v>
+        <v>1.29E-2</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" si="0"/>
-        <v>0.1996</v>
+        <v>2.58E-2</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>159</v>
+        <v>131</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="L13" t="str">
+        <v>200</v>
+      </c>
+      <c r="L13" s="20" t="str">
         <f>VLOOKUP(K13,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED RED DIFFUSED 0805 SMD</v>
+        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
       <c r="F14" s="17">
-        <v>0.1331</v>
+        <v>7.9899999999999999E-2</v>
       </c>
       <c r="G14" s="17">
         <f t="shared" si="0"/>
-        <v>0.26619999999999999</v>
+        <v>0.1598</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="L14" t="str">
+        <v>127</v>
+      </c>
+      <c r="L14" s="20" t="str">
         <f>VLOOKUP(K14,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED YELLOW DIFFUSED 0805 SMD</v>
+        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>235</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="17">
-        <v>0.13700000000000001</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="0"/>
-        <v>0.13700000000000001</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>156</v>
+        <v>221</v>
+      </c>
+      <c r="I15" s="2">
+        <v>691103110002</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>157</v>
+        <v>234</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="L15" t="str">
-        <f>VLOOKUP(K15,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED BLUE CLEAR 0805 SMD</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>83</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>82</v>
+        <v>232</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
       </c>
       <c r="F16" s="17">
-        <v>1.5347999999999999</v>
+        <v>9.9099999999999994E-2</v>
       </c>
       <c r="G16" s="17">
         <f t="shared" si="0"/>
-        <v>3.0695999999999999</v>
+        <v>0.19819999999999999</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>84</v>
+        <v>224</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>168</v>
+        <v>230</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>161</v>
+        <v>229</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="L16" t="str">
-        <f>VLOOKUP(K16,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
       </c>
       <c r="F17" s="17">
-        <v>6.7799999999999999E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="G17" s="17">
         <f t="shared" si="0"/>
-        <v>6.7799999999999999E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="L17" t="str">
+        <v>132</v>
+      </c>
+      <c r="L17" s="20" t="str">
         <f>VLOOKUP(K17,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>215</v>
+        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="17">
-        <v>0.62160000000000004</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="G18" s="17">
         <f t="shared" si="0"/>
-        <v>1.2432000000000001</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="L18" t="str">
+        <v>116</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" s="20" t="str">
         <f>VLOOKUP(K18,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
+        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" s="17">
-        <v>8.8000000000000005E-3</v>
+        <v>0.62160000000000004</v>
       </c>
       <c r="G19" s="17">
         <f t="shared" si="0"/>
-        <v>1.7600000000000001E-2</v>
+        <v>1.2432000000000001</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="L19" t="str">
+        <v>149</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L19" s="20" t="str">
         <f>VLOOKUP(K19,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
+        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
       </c>
       <c r="F20" s="17">
-        <v>0.60029999999999994</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="G20" s="17">
         <f t="shared" si="0"/>
-        <v>1.2005999999999999</v>
+        <v>8.8800000000000004E-2</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>125</v>
+        <v>218</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="L20" t="str">
+        <v>116</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="L20" s="20" t="str">
         <f>VLOOKUP(K20,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
+        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="17">
-        <v>0.4304</v>
+        <v>0.3019</v>
       </c>
       <c r="G21" s="17">
         <f t="shared" si="0"/>
-        <v>0.86080000000000001</v>
+        <v>0.3019</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>126</v>
+        <v>63</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="L21" t="str">
+        <v>152</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="L21" s="20" t="str">
         <f>VLOOKUP(K21,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
+        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="E22" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F22" s="17">
-        <v>1.29E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
-        <v>5.16E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="L22" t="str">
+        <v>139</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L22" s="20" t="str">
         <f>VLOOKUP(K22,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
+        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E23" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F23" s="17">
-        <v>8.6999999999999994E-3</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="G23" s="17">
         <f t="shared" si="0"/>
-        <v>8.6999999999999994E-2</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>222</v>
+        <v>69</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>117</v>
+        <v>156</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L23" t="str">
+        <v>155</v>
+      </c>
+      <c r="L23" s="20" t="str">
         <f>VLOOKUP(K23,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
+        <v>LED BLUE CLEAR 0805 SMD</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
-      </c>
-      <c r="F24" s="17">
-        <v>7.9899999999999999E-2</v>
-      </c>
-      <c r="G24" s="17">
-        <f t="shared" si="0"/>
-        <v>0.1598</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" t="str">
-        <f>VLOOKUP(K24,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
+        <v>73</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="M24" s="14" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="E25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="17">
-        <v>1.67E-2</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="G25" s="17">
-        <f t="shared" si="0"/>
-        <v>1.67E-2</v>
+        <f t="shared" ref="G25:G33" si="1">E25*F25</f>
+        <v>0.18959999999999999</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="L25" t="str">
+        <v>159</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="L25" s="20" t="str">
         <f>VLOOKUP(K25,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+        <v>LED GREEN DIFFUSED 0805 SMD</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" s="17">
-        <v>8.8000000000000005E-3</v>
+        <v>0.2437</v>
       </c>
       <c r="G26" s="17">
-        <f t="shared" si="0"/>
-        <v>8.8000000000000005E-3</v>
+        <f t="shared" si="1"/>
+        <v>0.73109999999999997</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>133</v>
+        <v>77</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="L26" t="str">
+        <v>154</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="L26" s="20" t="str">
         <f>VLOOKUP(K26,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
+        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="E27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="17">
-        <v>1.67E-2</v>
+        <v>1.5347999999999999</v>
       </c>
       <c r="G27" s="17">
-        <f t="shared" si="0"/>
-        <v>1.67E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.0695999999999999</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="L27" t="str">
+        <v>161</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="L27" s="20" t="str">
         <f>VLOOKUP(K27,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="E28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="17">
-        <v>1.29E-2</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="G28" s="17">
-        <f t="shared" si="0"/>
-        <v>2.58E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="L28" t="str">
+        <v>85</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="L28" s="20" t="str">
         <f>VLOOKUP(K28,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
+        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="E29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" s="17">
-        <v>8.8000000000000005E-3</v>
+        <v>9.98E-2</v>
       </c>
       <c r="G29" s="17">
-        <f t="shared" si="0"/>
-        <v>8.8000000000000005E-3</v>
+        <f t="shared" si="1"/>
+        <v>0.1996</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="L29" t="str">
+        <v>159</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L29" s="20" t="str">
         <f>VLOOKUP(K29,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
+        <v>LED RED DIFFUSED 0805 SMD</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="E30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" s="17">
-        <v>4.4400000000000002E-2</v>
+        <v>1.7770999999999999</v>
       </c>
       <c r="G30" s="17">
-        <f t="shared" si="0"/>
-        <v>8.8800000000000004E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.7770999999999999</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>219</v>
+        <v>96</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="L30" t="str">
+        <v>170</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="L30" s="20" t="str">
         <f>VLOOKUP(K30,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
+        <v>IC REG BOOST ADJ 2A SYNC 16VQFN</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>220</v>
+        <v>98</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="17">
-        <v>4.4400000000000002E-2</v>
+        <v>0.65680000000000005</v>
       </c>
       <c r="G31" s="17">
-        <f t="shared" si="0"/>
-        <v>4.4400000000000002E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.65680000000000005</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>139</v>
+        <v>228</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="L31" t="str">
-        <f>VLOOKUP(K31,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
+        <v>227</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="E32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" s="17">
-        <v>1.7770999999999999</v>
+        <v>0.1331</v>
       </c>
       <c r="G32" s="17">
-        <f t="shared" si="0"/>
-        <v>1.7770999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.26619999999999999</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>93</v>
+        <v>164</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="L32" t="str">
+        <v>163</v>
+      </c>
+      <c r="L32" s="20" t="str">
         <f>VLOOKUP(K32,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>IC REG BOOST ADJ 2A SYNC 16VQFN</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>LED YELLOW DIFFUSED 0805 SMD</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>102</v>
+        <v>236</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>99</v>
@@ -2560,67 +2513,73 @@
       <c r="D33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="2">
         <v>1</v>
       </c>
-      <c r="F33" s="17">
-        <v>0.65680000000000005</v>
+      <c r="F33" s="18">
+        <v>0.46920000000000001</v>
       </c>
       <c r="G33" s="17">
-        <f t="shared" si="0"/>
-        <v>0.65680000000000005</v>
+        <f t="shared" si="1"/>
+        <v>0.46920000000000001</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>101</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>228</v>
+        <v>237</v>
+      </c>
+      <c r="L33" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M33">
-    <sortState ref="A2:K42">
-      <sortCondition ref="A1:A42"/>
+  <autoFilter ref="A1:M32">
+    <sortState ref="A2:M32">
+      <sortCondition ref="D1:D32"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="K23" r:id="rId1"/>
-    <hyperlink ref="K22" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
-    <hyperlink ref="K20" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
-    <hyperlink ref="K21" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
-    <hyperlink ref="K24" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
-    <hyperlink ref="K28" r:id="rId6"/>
-    <hyperlink ref="K26" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
-    <hyperlink ref="K29" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
-    <hyperlink ref="K30" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
-    <hyperlink ref="K31" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
-    <hyperlink ref="K4" r:id="rId11" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM32ER61A107ME20L/490-9969-1-ND/5026474"/>
-    <hyperlink ref="K3" r:id="rId12"/>
-    <hyperlink ref="K5" r:id="rId13" display="https://www.digikey.com/product-detail/en/yageo/CC0805ZRY5V9BB104/311-1361-1-ND/2103145"/>
-    <hyperlink ref="K7" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
-    <hyperlink ref="K18" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
-    <hyperlink ref="K10" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
-    <hyperlink ref="K8" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
-    <hyperlink ref="K12" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
-    <hyperlink ref="K13" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
-    <hyperlink ref="K14" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
-    <hyperlink ref="K15" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
-    <hyperlink ref="K16" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
-    <hyperlink ref="K32" r:id="rId23"/>
-    <hyperlink ref="K27" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="K25" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="K19" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
-    <hyperlink ref="K17" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
-    <hyperlink ref="K6" r:id="rId28"/>
-    <hyperlink ref="K33" r:id="rId29"/>
-    <hyperlink ref="K11" r:id="rId30"/>
-    <hyperlink ref="K2" r:id="rId31"/>
+    <hyperlink ref="K11" r:id="rId1"/>
+    <hyperlink ref="K5" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
+    <hyperlink ref="K9" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
+    <hyperlink ref="K10" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
+    <hyperlink ref="K14" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
+    <hyperlink ref="K13" r:id="rId6"/>
+    <hyperlink ref="K17" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
+    <hyperlink ref="K18" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
+    <hyperlink ref="K20" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
+    <hyperlink ref="K22" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
+    <hyperlink ref="K6" r:id="rId11" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM32ER61A107ME20L/490-9969-1-ND/5026474"/>
+    <hyperlink ref="K8" r:id="rId12"/>
+    <hyperlink ref="K2" r:id="rId13" display="https://www.digikey.com/product-detail/en/yageo/CC0805ZRY5V9BB104/311-1361-1-ND/2103145"/>
+    <hyperlink ref="K12" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
+    <hyperlink ref="K19" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
+    <hyperlink ref="K21" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
+    <hyperlink ref="K26" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
+    <hyperlink ref="K25" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
+    <hyperlink ref="K29" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
+    <hyperlink ref="K32" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
+    <hyperlink ref="K23" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
+    <hyperlink ref="K27" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
+    <hyperlink ref="K30" r:id="rId23"/>
+    <hyperlink ref="K3" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K4" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K7" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
+    <hyperlink ref="K28" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
+    <hyperlink ref="K31" r:id="rId28"/>
+    <hyperlink ref="K16" r:id="rId29"/>
+    <hyperlink ref="K15" r:id="rId30"/>
+    <hyperlink ref="K33" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId32"/>
@@ -2638,35 +2597,37 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>178</v>
-      </c>
-      <c r="C1" t="s">
-        <v>179</v>
       </c>
       <c r="D1" t="s">
         <v>104</v>
       </c>
       <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>182</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>183</v>
-      </c>
-      <c r="I1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2680,7 +2641,7 @@
         <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -2706,7 +2667,7 @@
         <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -2732,7 +2693,7 @@
         <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -2758,7 +2719,7 @@
         <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -2784,7 +2745,7 @@
         <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -2810,7 +2771,7 @@
         <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -2836,7 +2797,7 @@
         <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -2862,7 +2823,7 @@
         <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -2888,7 +2849,7 @@
         <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -2914,7 +2875,7 @@
         <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -2940,7 +2901,7 @@
         <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -2966,7 +2927,7 @@
         <v>167</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -2989,10 +2950,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3018,7 +2979,7 @@
         <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3044,7 +3005,7 @@
         <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3070,7 +3031,7 @@
         <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3093,10 +3054,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
         <v>201</v>
-      </c>
-      <c r="D18" t="s">
-        <v>202</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3122,7 +3083,7 @@
         <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3148,7 +3109,7 @@
         <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3171,10 +3132,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3200,7 +3161,7 @@
         <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -3226,7 +3187,7 @@
         <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -3252,7 +3213,7 @@
         <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -3278,7 +3239,7 @@
         <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -3301,10 +3262,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -3330,7 +3291,7 @@
         <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F27">
         <v>10</v>
@@ -3356,7 +3317,7 @@
         <v>150</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -3379,10 +3340,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F29">
         <v>10</v>
@@ -3420,31 +3381,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>178</v>
-      </c>
-      <c r="C1" t="s">
-        <v>179</v>
       </c>
       <c r="D1" t="s">
         <v>104</v>
       </c>
       <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>182</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>183</v>
-      </c>
-      <c r="I1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3458,7 +3419,7 @@
         <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -3484,7 +3445,7 @@
         <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -3510,7 +3471,7 @@
         <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -3536,7 +3497,7 @@
         <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -3562,7 +3523,7 @@
         <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -3588,7 +3549,7 @@
         <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -3614,7 +3575,7 @@
         <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -3640,7 +3601,7 @@
         <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -3666,7 +3627,7 @@
         <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -3692,7 +3653,7 @@
         <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -3718,7 +3679,7 @@
         <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3744,7 +3705,7 @@
         <v>167</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3767,10 +3728,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3796,7 +3757,7 @@
         <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3822,7 +3783,7 @@
         <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3848,7 +3809,7 @@
         <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3871,10 +3832,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
         <v>201</v>
-      </c>
-      <c r="D18" t="s">
-        <v>202</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3900,7 +3861,7 @@
         <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3926,7 +3887,7 @@
         <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3949,10 +3910,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3978,7 +3939,7 @@
         <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -4004,7 +3965,7 @@
         <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -4030,7 +3991,7 @@
         <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -4056,7 +4017,7 @@
         <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -4079,10 +4040,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -4108,7 +4069,7 @@
         <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F27">
         <v>10</v>

</xml_diff>

<commit_message>
Updated BOM and layout for LTC4015
Schematic pinout redone for LTC4015 part to match design application guide and make schematic easier to follow. Schematic and board routing started. BOM updated and consolidated for last revision of board (non-LTC)
</commit_message>
<xml_diff>
--- a/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
+++ b/BOM/BOM_Main_Board_2X-SOLAR_5V-DCDC_digikey.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$M$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="236">
   <si>
     <t>Qty</t>
   </si>
@@ -530,9 +530,6 @@
     <t>MCP73871-2CCI/ML</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>296-15259-1-ND</t>
   </si>
   <si>
@@ -684,9 +681,6 @@
   </si>
   <si>
     <t>75K</t>
-  </si>
-  <si>
-    <t>C15</t>
   </si>
   <si>
     <t>R7, R8, R9, R10, R13, R14, R11, R15, R39, R40</t>
@@ -744,7 +738,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,45 +808,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -875,7 +830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -930,25 +885,6 @@
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1257,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>103</v>
@@ -1315,10 +1251,10 @@
         <v>108</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1332,7 +1268,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1345,16 +1281,16 @@
         <v>0.57099999999999995</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I2" s="2">
         <v>691103110002</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1381,7 +1317,7 @@
         <v>0.56420000000000003</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>111</v>
@@ -1477,231 +1413,231 @@
         <v>CAP CER 0.1UF 50V Y5V 0805</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="20">
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="L6" s="24" t="str">
+      <c r="F6" s="17">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="G6" s="17">
+        <f>E6*F6</f>
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" t="str">
         <f>VLOOKUP(K6,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 10UF 16V X5R 0805</v>
-      </c>
-      <c r="M6" s="25"/>
+        <v>CAP CER 2.2UF 25V X5R 0805</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="17">
-        <v>3.9399999999999998E-2</v>
+        <v>0.2437</v>
       </c>
       <c r="G7" s="17">
         <f>E7*F7</f>
-        <v>3.9399999999999998E-2</v>
+        <v>0.73109999999999997</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="L7" t="str">
         <f>VLOOKUP(K7,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP CER 2.2UF 25V X5R 0805</v>
+        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="F8" s="17">
-        <v>0.2437</v>
-      </c>
-      <c r="G8" s="17">
-        <f>E8*F8</f>
-        <v>0.73109999999999997</v>
-      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="L8" t="str">
-        <f>VLOOKUP(K8,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>DIODE SCHOTTKY 20V 1A SOD123FL</v>
+        <v>73</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="M8" s="14" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1">
-        <v>3</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.3019</v>
+      </c>
+      <c r="G9" s="17">
+        <f>E9*F9</f>
+        <v>0.3019</v>
+      </c>
       <c r="H9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="M9" s="14" t="s">
-        <v>216</v>
+        <v>63</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="L9" t="str">
+        <f>VLOOKUP(K9,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>232</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="17">
-        <v>0.3019</v>
+        <v>9.9099999999999994E-2</v>
       </c>
       <c r="G10" s="17">
         <f>E10*F10</f>
-        <v>0.3019</v>
+        <v>0.19819999999999999</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>151</v>
+        <v>230</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="L10" t="str">
-        <f>VLOOKUP(K10,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>FIXED IND 6.8UH 2.9A 59.8 MOHM</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>213</v>
+        <v>229</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>234</v>
+        <v>75</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="17">
-        <v>9.9099999999999994E-2</v>
+        <v>9.4799999999999995E-2</v>
       </c>
       <c r="G11" s="17">
-        <f>E11*F11</f>
-        <v>0.19819999999999999</v>
+        <f t="shared" ref="G11:G32" si="0">E11*F11</f>
+        <v>0.18959999999999999</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>226</v>
+        <v>76</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>231</v>
+        <v>159</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>233</v>
+        <v>158</v>
+      </c>
+      <c r="L11" t="str">
+        <f>VLOOKUP(K11,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
+        <v>LED GREEN DIFFUSED 0805 SMD</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1715,33 +1651,33 @@
         <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
       </c>
       <c r="F12" s="17">
-        <v>9.4799999999999995E-2</v>
+        <v>9.98E-2</v>
       </c>
       <c r="G12" s="17">
-        <f t="shared" ref="G12:G33" si="0">E12*F12</f>
-        <v>0.18959999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.1996</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>159</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="L12" t="str">
         <f>VLOOKUP(K12,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED GREEN DIFFUSED 0805 SMD</v>
+        <v>LED RED DIFFUSED 0805 SMD</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1755,33 +1691,33 @@
         <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="17">
-        <v>9.98E-2</v>
+        <v>0.1331</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" si="0"/>
-        <v>0.1996</v>
+        <v>0.26619999999999999</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>159</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L13" t="str">
         <f>VLOOKUP(K13,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED RED DIFFUSED 0805 SMD</v>
+        <v>LED YELLOW DIFFUSED 0805 SMD</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1795,239 +1731,239 @@
         <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>165</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="17">
-        <v>0.1331</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="G14" s="17">
         <f t="shared" si="0"/>
-        <v>0.26619999999999999</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="L14" t="str">
         <f>VLOOKUP(K14,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED YELLOW DIFFUSED 0805 SMD</v>
+        <v>LED BLUE CLEAR 0805 SMD</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="17">
-        <v>0.13700000000000001</v>
+        <v>1.5347999999999999</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="0"/>
-        <v>0.13700000000000001</v>
+        <v>3.0695999999999999</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="L15" t="str">
         <f>VLOOKUP(K15,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>LED BLUE CLEAR 0805 SMD</v>
+        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="17">
-        <v>1.5347999999999999</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="G16" s="17">
         <f t="shared" si="0"/>
-        <v>3.0695999999999999</v>
+        <v>6.7799999999999999E-2</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>167</v>
+        <v>154</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>213</v>
       </c>
       <c r="L16" t="str">
         <f>VLOOKUP(K16,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>IC USB/AC BATT CHRGR W/PPM 20QFN</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="17">
-        <v>6.7799999999999999E-2</v>
+        <v>0.62160000000000004</v>
       </c>
       <c r="G17" s="17">
         <f t="shared" si="0"/>
-        <v>6.7799999999999999E-2</v>
+        <v>1.2432000000000001</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>214</v>
+        <v>149</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="L17" t="str">
         <f>VLOOKUP(K17,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>TRANS PREBIAS PNP 246MW SOT23-3</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
       </c>
       <c r="F18" s="17">
-        <v>0.62160000000000004</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="G18" s="17">
         <f t="shared" si="0"/>
-        <v>1.2432000000000001</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>147</v>
+        <v>116</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="L18" t="str">
         <f>VLOOKUP(K18,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>CAP ALUM 4700UF 20% 10V RADIAL</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
       </c>
       <c r="F19" s="17">
-        <v>8.8000000000000005E-3</v>
+        <v>0.60029999999999994</v>
       </c>
       <c r="G19" s="17">
         <f t="shared" si="0"/>
-        <v>1.7600000000000001E-2</v>
+        <v>1.2005999999999999</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>175</v>
+        <v>41</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>125</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>174</v>
+        <v>124</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="L19" t="str">
         <f>VLOOKUP(K19,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 10K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2038,76 +1974,76 @@
         <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
       </c>
       <c r="F20" s="17">
-        <v>0.60029999999999994</v>
+        <v>0.4304</v>
       </c>
       <c r="G20" s="17">
         <f t="shared" si="0"/>
-        <v>1.2005999999999999</v>
+        <v>0.86080000000000001</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L20" t="str">
         <f>VLOOKUP(K20,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 150K OHM 0.05% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" s="17">
-        <v>0.4304</v>
+        <v>1.29E-2</v>
       </c>
       <c r="G21" s="17">
         <f t="shared" si="0"/>
-        <v>0.86080000000000001</v>
+        <v>5.16E-2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>116</v>
+        <v>24</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L21" t="str">
         <f>VLOOKUP(K21,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 0.1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -2118,36 +2054,36 @@
         <v>8</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F22" s="17">
-        <v>1.29E-2</v>
+        <v>8.6999999999999994E-3</v>
       </c>
       <c r="G22" s="17">
         <f t="shared" si="0"/>
-        <v>5.16E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>24</v>
+        <v>220</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>117</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="L22" t="str">
         <f>VLOOKUP(K22,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 100K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2158,76 +2094,76 @@
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F23" s="17">
-        <v>8.6999999999999994E-3</v>
+        <v>7.9899999999999999E-2</v>
       </c>
       <c r="G23" s="17">
         <f t="shared" si="0"/>
-        <v>8.6999999999999994E-2</v>
+        <v>0.1598</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>222</v>
+        <v>49</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>117</v>
+        <v>129</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="L23" t="str">
         <f>VLOOKUP(K23,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1K OHM 5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="E24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="17">
-        <v>7.9899999999999999E-2</v>
+        <v>1.67E-2</v>
       </c>
       <c r="G24" s="17">
         <f t="shared" si="0"/>
-        <v>0.1598</v>
+        <v>1.67E-2</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>127</v>
+      <c r="K24" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="L24" t="str">
         <f>VLOOKUP(K24,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 270K OHM 0.5% 1/4W 0805</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
@@ -2238,76 +2174,76 @@
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25" s="17">
-        <v>1.67E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="G25" s="17">
         <f t="shared" si="0"/>
-        <v>1.67E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>172</v>
+        <v>132</v>
       </c>
       <c r="L25" t="str">
         <f>VLOOKUP(K25,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
       </c>
       <c r="F26" s="17">
-        <v>8.8000000000000005E-3</v>
+        <v>1.67E-2</v>
       </c>
       <c r="G26" s="17">
         <f t="shared" si="0"/>
-        <v>8.8000000000000005E-3</v>
+        <v>1.67E-2</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="L26" t="str">
         <f>VLOOKUP(K26,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 340K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
@@ -2318,36 +2254,36 @@
         <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="17">
-        <v>1.67E-2</v>
+        <v>1.29E-2</v>
       </c>
       <c r="G27" s="17">
         <f t="shared" si="0"/>
-        <v>1.67E-2</v>
+        <v>2.58E-2</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>172</v>
+        <v>131</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>200</v>
       </c>
       <c r="L27" t="str">
         <f>VLOOKUP(K27,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 1.87M OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>19</v>
       </c>
@@ -2358,36 +2294,36 @@
         <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28" s="17">
-        <v>1.29E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="G28" s="17">
         <f t="shared" si="0"/>
-        <v>2.58E-2</v>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>201</v>
+        <v>135</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="L28" t="str">
         <f>VLOOKUP(K28,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 200K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>19</v>
       </c>
@@ -2398,36 +2334,36 @@
         <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" s="17">
-        <v>8.8000000000000005E-3</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="G29" s="17">
         <f t="shared" si="0"/>
-        <v>8.8000000000000005E-3</v>
+        <v>8.8800000000000004E-2</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>116</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L29" t="str">
         <f>VLOOKUP(K29,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 43K OHM 1% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>19</v>
       </c>
@@ -2438,192 +2374,151 @@
         <v>17</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="E30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" s="17">
         <v>4.4400000000000002E-2</v>
       </c>
       <c r="G30" s="17">
         <f t="shared" si="0"/>
-        <v>8.8800000000000004E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>219</v>
+        <v>65</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>116</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L30" t="str">
         <f>VLOOKUP(K30,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 49.9K OHM 0.5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>220</v>
+        <v>93</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="17">
-        <v>4.4400000000000002E-2</v>
+        <v>1.7770999999999999</v>
       </c>
       <c r="G31" s="17">
         <f t="shared" si="0"/>
-        <v>4.4400000000000002E-2</v>
+        <v>1.7770999999999999</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>138</v>
+        <v>170</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="L31" t="str">
         <f>VLOOKUP(K31,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>RES SMD 75K OHM 0.5% 1/8W 0805</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>IC REG BOOST ADJ 2A SYNC 16VQFN</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E32" s="1">
         <v>1</v>
       </c>
       <c r="F32" s="17">
-        <v>1.7770999999999999</v>
+        <v>0.65680000000000005</v>
       </c>
       <c r="G32" s="17">
         <f t="shared" si="0"/>
-        <v>1.7770999999999999</v>
+        <v>0.65680000000000005</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>93</v>
+        <v>228</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="L32" t="str">
-        <f>VLOOKUP(K32,'2017-06-07T13-52-05'!$C$2:$J$29,2,FALSE)</f>
-        <v>IC REG BOOST ADJ 2A SYNC 16VQFN</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="17">
-        <v>0.65680000000000005</v>
-      </c>
-      <c r="G33" s="17">
-        <f t="shared" si="0"/>
-        <v>0.65680000000000005</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M33">
+  <autoFilter ref="A1:M32">
     <sortState ref="A2:K42">
       <sortCondition ref="A1:A42"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="K23" r:id="rId1"/>
-    <hyperlink ref="K22" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
-    <hyperlink ref="K20" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
-    <hyperlink ref="K21" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
-    <hyperlink ref="K24" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
-    <hyperlink ref="K28" r:id="rId6"/>
-    <hyperlink ref="K26" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
-    <hyperlink ref="K29" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
-    <hyperlink ref="K30" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
-    <hyperlink ref="K31" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
+    <hyperlink ref="K22" r:id="rId1"/>
+    <hyperlink ref="K21" r:id="rId2" display="https://www.digikey.com/product-detail/en/bourns-inc/CR0805-FX-1003ELF/CR0805-FX-1003ELFCT-ND/3740923"/>
+    <hyperlink ref="K19" r:id="rId3" display="https://www.digikey.com/product-detail/en/susumu/RG2012N-154-W-T1/RG20N150KWCT-ND/600928"/>
+    <hyperlink ref="K20" r:id="rId4" display="https://www.digikey.com/product-detail/en/yageo/RT0805BRB071KL/YAG4811CT-ND/6616967"/>
+    <hyperlink ref="K23" r:id="rId5" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-PB6D2703V/P21294CT-ND/6215549"/>
+    <hyperlink ref="K27" r:id="rId6"/>
+    <hyperlink ref="K25" r:id="rId7" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-07340KL/311-340KCRCT-ND/730822"/>
+    <hyperlink ref="K28" r:id="rId8" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0743KL/311-43.0KCRCT-ND/730900"/>
+    <hyperlink ref="K29" r:id="rId9" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRE0749K9L/311-2869-1-ND/6129288"/>
+    <hyperlink ref="K30" r:id="rId10" display="https://www.digikey.com/product-detail/en/yageo/RT0805DRD0775KL/311-2766-1-ND/6129185"/>
     <hyperlink ref="K4" r:id="rId11" display="https://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM32ER61A107ME20L/490-9969-1-ND/5026474"/>
     <hyperlink ref="K3" r:id="rId12"/>
     <hyperlink ref="K5" r:id="rId13" display="https://www.digikey.com/product-detail/en/yageo/CC0805ZRY5V9BB104/311-1361-1-ND/2103145"/>
-    <hyperlink ref="K7" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
-    <hyperlink ref="K18" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
-    <hyperlink ref="K10" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
-    <hyperlink ref="K8" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
-    <hyperlink ref="K12" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
-    <hyperlink ref="K13" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
-    <hyperlink ref="K14" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
-    <hyperlink ref="K15" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
-    <hyperlink ref="K16" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
-    <hyperlink ref="K32" r:id="rId23"/>
-    <hyperlink ref="K27" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="K25" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
-    <hyperlink ref="K19" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
-    <hyperlink ref="K17" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
-    <hyperlink ref="K6" r:id="rId28"/>
-    <hyperlink ref="K33" r:id="rId29"/>
-    <hyperlink ref="K11" r:id="rId30"/>
-    <hyperlink ref="K2" r:id="rId31"/>
+    <hyperlink ref="K6" r:id="rId14" display="https://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL21A225KAFNNNG/1276-6458-1-ND/5958086"/>
+    <hyperlink ref="K17" r:id="rId15" display="https://www.digikey.com/product-detail/en/nichicon/UVR1A472MHD1TO/493-12761-1-ND/4328397"/>
+    <hyperlink ref="K9" r:id="rId16" display="https://www.digikey.com/product-detail/en/tdk-corporation/VLS5045EX-6R8M/445-174855-1-ND/6560412"/>
+    <hyperlink ref="K7" r:id="rId17" display="https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT1G/MBR120VLSFT1GOSCT-ND/893874"/>
+    <hyperlink ref="K11" r:id="rId18" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-R971-KN-1/475-1410-1-ND/1802598"/>
+    <hyperlink ref="K12" r:id="rId19" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LS-R976-NR-1/475-1278-1-ND/1642798"/>
+    <hyperlink ref="K13" r:id="rId20" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LY-R976-PS-36/475-2560-1-ND/1802687"/>
+    <hyperlink ref="K14" r:id="rId21" display="https://www.digikey.com/product-detail/en/wurth-electronics-inc/150080BS75000/732-4982-1-ND/4489910"/>
+    <hyperlink ref="K15" r:id="rId22" display="https://www.digikey.com/product-detail/en/microchip-technology/MCP73871-2CCI-ML/MCP73871-2CCI-ML-ND/1680971"/>
+    <hyperlink ref="K31" r:id="rId23"/>
+    <hyperlink ref="K26" r:id="rId24" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K24" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-6ENF1874V/P1.87BTCT-ND/4429149"/>
+    <hyperlink ref="K18" r:id="rId26" display="https://www.digikey.com/product-detail/en/yageo/RC0805FR-0710KL/311-10.0KCRCT-ND/730482"/>
+    <hyperlink ref="K16" r:id="rId27" display="https://www.digikey.com/product-detail/en/on-semiconductor/MMUN2133LT1G/MMUN2133LT1GOSCT-ND/2705149"/>
+    <hyperlink ref="K32" r:id="rId28"/>
+    <hyperlink ref="K10" r:id="rId29"/>
+    <hyperlink ref="K2" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -2642,31 +2537,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>178</v>
-      </c>
-      <c r="C1" t="s">
-        <v>179</v>
       </c>
       <c r="D1" t="s">
         <v>104</v>
       </c>
       <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>182</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>183</v>
-      </c>
-      <c r="I1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2680,7 +2575,7 @@
         <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -2706,7 +2601,7 @@
         <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -2732,7 +2627,7 @@
         <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -2758,7 +2653,7 @@
         <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -2784,7 +2679,7 @@
         <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -2810,7 +2705,7 @@
         <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -2836,7 +2731,7 @@
         <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -2862,7 +2757,7 @@
         <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -2888,7 +2783,7 @@
         <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -2914,7 +2809,7 @@
         <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -2940,7 +2835,7 @@
         <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -2966,7 +2861,7 @@
         <v>167</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -2989,10 +2884,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3018,7 +2913,7 @@
         <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3044,7 +2939,7 @@
         <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3070,7 +2965,7 @@
         <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3093,10 +2988,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
         <v>201</v>
-      </c>
-      <c r="D18" t="s">
-        <v>202</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3122,7 +3017,7 @@
         <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3148,7 +3043,7 @@
         <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3171,10 +3066,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3200,7 +3095,7 @@
         <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -3226,7 +3121,7 @@
         <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -3252,7 +3147,7 @@
         <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -3278,7 +3173,7 @@
         <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -3301,10 +3196,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -3330,7 +3225,7 @@
         <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F27">
         <v>10</v>
@@ -3356,7 +3251,7 @@
         <v>150</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -3379,10 +3274,10 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F29">
         <v>10</v>
@@ -3420,31 +3315,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>178</v>
-      </c>
-      <c r="C1" t="s">
-        <v>179</v>
       </c>
       <c r="D1" t="s">
         <v>104</v>
       </c>
       <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>181</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>182</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>183</v>
-      </c>
-      <c r="I1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3458,7 +3353,7 @@
         <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -3484,7 +3379,7 @@
         <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -3510,7 +3405,7 @@
         <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -3536,7 +3431,7 @@
         <v>121</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5">
         <v>12</v>
@@ -3562,7 +3457,7 @@
         <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6">
         <v>10</v>
@@ -3588,7 +3483,7 @@
         <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -3614,7 +3509,7 @@
         <v>158</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -3640,7 +3535,7 @@
         <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F9">
         <v>10</v>
@@ -3666,7 +3561,7 @@
         <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10">
         <v>10</v>
@@ -3692,7 +3587,7 @@
         <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -3718,7 +3613,7 @@
         <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F12">
         <v>6</v>
@@ -3744,7 +3639,7 @@
         <v>167</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13">
         <v>6</v>
@@ -3767,10 +3662,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -3796,7 +3691,7 @@
         <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -3822,7 +3717,7 @@
         <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16">
         <v>10</v>
@@ -3848,7 +3743,7 @@
         <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F17">
         <v>10</v>
@@ -3871,10 +3766,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" t="s">
         <v>201</v>
-      </c>
-      <c r="D18" t="s">
-        <v>202</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -3900,7 +3795,7 @@
         <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F19">
         <v>10</v>
@@ -3926,7 +3821,7 @@
         <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F20">
         <v>10</v>
@@ -3949,10 +3844,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F21">
         <v>10</v>
@@ -3978,7 +3873,7 @@
         <v>132</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -4004,7 +3899,7 @@
         <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F23">
         <v>10</v>
@@ -4030,7 +3925,7 @@
         <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -4056,7 +3951,7 @@
         <v>138</v>
       </c>
       <c r="D25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -4079,10 +3974,10 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -4108,7 +4003,7 @@
         <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F27">
         <v>10</v>

</xml_diff>